<commit_message>
Fixed averaging bug Where it would be a static index B and not dynamic for each column
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,6 +9,8 @@
     <sheet name="120mm_8deg_trial1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="120mm_20deg_trial1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="120mm_20deg_trial2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="120mm_20deg_trial3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="120mm_20deg_trial4" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -16109,7 +16111,6 @@
       <c r="CJ3" t="n">
         <v>180</v>
       </c>
-      <c r="CK3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -16274,7 +16275,6 @@
       <c r="CJ4" t="n">
         <v>180</v>
       </c>
-      <c r="CK4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -16439,7 +16439,6 @@
       <c r="CJ5" t="n">
         <v>180</v>
       </c>
-      <c r="CK5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -16604,7 +16603,6 @@
       <c r="CJ6" t="n">
         <v>180</v>
       </c>
-      <c r="CK6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -16769,7 +16767,6 @@
       <c r="CJ7" t="n">
         <v>180</v>
       </c>
-      <c r="CK7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -16934,7 +16931,6 @@
       <c r="CJ8" t="n">
         <v>180</v>
       </c>
-      <c r="CK8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -17099,7 +17095,6 @@
       <c r="CJ9" t="n">
         <v>180</v>
       </c>
-      <c r="CK9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -17264,7 +17259,6 @@
       <c r="CJ10" t="n">
         <v>180</v>
       </c>
-      <c r="CK10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -17429,7 +17423,6 @@
       <c r="CJ11" t="n">
         <v>180</v>
       </c>
-      <c r="CK11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -17594,7 +17587,6 @@
       <c r="CJ12" t="n">
         <v>180</v>
       </c>
-      <c r="CK12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -17759,7 +17751,6 @@
       <c r="CJ13" t="n">
         <v>180</v>
       </c>
-      <c r="CK13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -17924,7 +17915,6 @@
       <c r="CJ14" t="n">
         <v>180</v>
       </c>
-      <c r="CK14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -18089,7 +18079,6 @@
       <c r="CJ15" t="n">
         <v>180</v>
       </c>
-      <c r="CK15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -18254,7 +18243,6 @@
       <c r="CJ16" t="n">
         <v>180</v>
       </c>
-      <c r="CK16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -18419,7 +18407,6 @@
       <c r="CJ17" t="n">
         <v>180</v>
       </c>
-      <c r="CK17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -18584,7 +18571,6 @@
       <c r="CJ18" t="n">
         <v>180</v>
       </c>
-      <c r="CK18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -18749,7 +18735,6 @@
       <c r="CJ19" t="n">
         <v>180</v>
       </c>
-      <c r="CK19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -18914,7 +18899,6 @@
       <c r="CJ20" t="n">
         <v>180</v>
       </c>
-      <c r="CK20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -19079,7 +19063,6 @@
       <c r="CJ21" t="n">
         <v>180</v>
       </c>
-      <c r="CK21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -19244,7 +19227,6 @@
       <c r="CJ22" t="n">
         <v>180</v>
       </c>
-      <c r="CK22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -19409,7 +19391,6 @@
       <c r="CJ23" t="n">
         <v>180</v>
       </c>
-      <c r="CK23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -19574,7 +19555,6 @@
       <c r="CJ24" t="n">
         <v>180</v>
       </c>
-      <c r="CK24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -19739,7 +19719,6 @@
       <c r="CJ25" t="n">
         <v>180</v>
       </c>
-      <c r="CK25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -19904,7 +19883,6 @@
       <c r="CJ26" t="n">
         <v>180</v>
       </c>
-      <c r="CK26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -20069,7 +20047,6 @@
       <c r="CJ27" t="n">
         <v>180</v>
       </c>
-      <c r="CK27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -20234,7 +20211,6 @@
       <c r="CJ28" t="n">
         <v>180</v>
       </c>
-      <c r="CK28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -20399,7 +20375,6 @@
       <c r="CJ29" t="n">
         <v>180</v>
       </c>
-      <c r="CK29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -20564,7 +20539,6 @@
       <c r="CJ30" t="n">
         <v>180</v>
       </c>
-      <c r="CK30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -20729,7 +20703,6 @@
       <c r="CJ31" t="n">
         <v>180</v>
       </c>
-      <c r="CK31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -20894,7 +20867,6 @@
       <c r="CJ32" t="n">
         <v>180</v>
       </c>
-      <c r="CK32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -21059,7 +21031,6 @@
       <c r="CJ33" t="n">
         <v>180</v>
       </c>
-      <c r="CK33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -21224,7 +21195,6 @@
       <c r="CJ34" t="n">
         <v>180</v>
       </c>
-      <c r="CK34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -21389,7 +21359,6 @@
       <c r="CJ35" t="n">
         <v>180</v>
       </c>
-      <c r="CK35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -21554,7 +21523,6 @@
       <c r="CJ36" t="n">
         <v>180</v>
       </c>
-      <c r="CK36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -21719,7 +21687,6 @@
       <c r="CJ37" t="n">
         <v>180</v>
       </c>
-      <c r="CK37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -21884,7 +21851,6 @@
       <c r="CJ38" t="n">
         <v>180</v>
       </c>
-      <c r="CK38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -22049,7 +22015,6 @@
       <c r="CJ39" t="n">
         <v>180</v>
       </c>
-      <c r="CK39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -22214,7 +22179,6 @@
       <c r="CJ40" t="n">
         <v>180</v>
       </c>
-      <c r="CK40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -22379,7 +22343,6 @@
       <c r="CJ41" t="n">
         <v>180</v>
       </c>
-      <c r="CK41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -22544,7 +22507,6 @@
       <c r="CJ42" t="n">
         <v>180</v>
       </c>
-      <c r="CK42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -22709,7 +22671,6 @@
       <c r="CJ43" t="n">
         <v>180</v>
       </c>
-      <c r="CK43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -22874,7 +22835,6 @@
       <c r="CJ44" t="n">
         <v>180</v>
       </c>
-      <c r="CK44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -23039,7 +22999,6 @@
       <c r="CJ45" t="n">
         <v>180</v>
       </c>
-      <c r="CK45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -23204,7 +23163,6 @@
       <c r="CJ46" t="n">
         <v>180</v>
       </c>
-      <c r="CK46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -23369,7 +23327,6 @@
       <c r="CJ47" t="n">
         <v>180</v>
       </c>
-      <c r="CK47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -23534,7 +23491,6 @@
       <c r="CJ48" t="n">
         <v>180</v>
       </c>
-      <c r="CK48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -23699,7 +23655,6 @@
       <c r="CJ49" t="n">
         <v>180</v>
       </c>
-      <c r="CK49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -23864,7 +23819,3082 @@
       <c r="CJ50" t="n">
         <v>180</v>
       </c>
-      <c r="CK50" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Throttle</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Throttle</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.192092895507812e-06</v>
+      </c>
+      <c r="B2" t="n">
+        <v>4.16076</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGE(C$2:C$10000)</f>
+        <v/>
+      </c>
+      <c r="F2" t="n">
+        <v>9.5367431640625e-07</v>
+      </c>
+      <c r="G2" t="n">
+        <v>7.69958</v>
+      </c>
+      <c r="H2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(C$2:C$10000)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0.1063871383666992</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4.16076</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.1073760986328125</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7.69594</v>
+      </c>
+      <c r="H3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.2046051025390625</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4.16803</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.2087619304656982</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7.69594</v>
+      </c>
+      <c r="H4" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.3216221332550049</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4.16803</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.3204431533813477</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7.70322</v>
+      </c>
+      <c r="H5" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.4217653274536133</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4.17167</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.4220221042633057</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7.69958</v>
+      </c>
+      <c r="H6" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.5269181728363037</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4.17167</v>
+      </c>
+      <c r="C7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.5236678123474121</v>
+      </c>
+      <c r="G7" t="n">
+        <v>7.69231</v>
+      </c>
+      <c r="H7" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.6362261772155762</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4.16803</v>
+      </c>
+      <c r="C8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.6283049583435059</v>
+      </c>
+      <c r="G8" t="n">
+        <v>7.67776</v>
+      </c>
+      <c r="H8" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.7380132675170898</v>
+      </c>
+      <c r="B9" t="n">
+        <v>4.16439</v>
+      </c>
+      <c r="C9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.7377369403839111</v>
+      </c>
+      <c r="G9" t="n">
+        <v>7.66685</v>
+      </c>
+      <c r="H9" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.8415753841400146</v>
+      </c>
+      <c r="B10" t="n">
+        <v>4.16803</v>
+      </c>
+      <c r="C10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.8401651382446289</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7.66321</v>
+      </c>
+      <c r="H10" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.9424262046813965</v>
+      </c>
+      <c r="B11" t="n">
+        <v>4.16803</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9441769123077393</v>
+      </c>
+      <c r="G11" t="n">
+        <v>7.65594</v>
+      </c>
+      <c r="H11" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.053994178771973</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4.14984</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.054631948471069</v>
+      </c>
+      <c r="G12" t="n">
+        <v>7.65594</v>
+      </c>
+      <c r="H12" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1.155270338058472</v>
+      </c>
+      <c r="B13" t="n">
+        <v>4.14621</v>
+      </c>
+      <c r="C13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.153992891311646</v>
+      </c>
+      <c r="G13" t="n">
+        <v>7.65957</v>
+      </c>
+      <c r="H13" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.260323286056519</v>
+      </c>
+      <c r="B14" t="n">
+        <v>4.13893</v>
+      </c>
+      <c r="C14" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.257920026779175</v>
+      </c>
+      <c r="G14" t="n">
+        <v>7.66321</v>
+      </c>
+      <c r="H14" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.369219064712524</v>
+      </c>
+      <c r="B15" t="n">
+        <v>4.12802</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.361820936203003</v>
+      </c>
+      <c r="G15" t="n">
+        <v>7.65957</v>
+      </c>
+      <c r="H15" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.472801208496094</v>
+      </c>
+      <c r="B16" t="n">
+        <v>4.11347</v>
+      </c>
+      <c r="C16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.47339391708374</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7.65594</v>
+      </c>
+      <c r="H16" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.574851274490356</v>
+      </c>
+      <c r="B17" t="n">
+        <v>4.09893</v>
+      </c>
+      <c r="C17" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.574110984802246</v>
+      </c>
+      <c r="G17" t="n">
+        <v>7.65594</v>
+      </c>
+      <c r="H17" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.680556058883667</v>
+      </c>
+      <c r="B18" t="n">
+        <v>4.08438</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.67866587638855</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7.66321</v>
+      </c>
+      <c r="H18" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.785797119140625</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4.07347</v>
+      </c>
+      <c r="C19" t="n">
+        <v>10</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.79155707359314</v>
+      </c>
+      <c r="G19" t="n">
+        <v>7.6523</v>
+      </c>
+      <c r="H19" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.889755249023438</v>
+      </c>
+      <c r="B20" t="n">
+        <v>4.06983</v>
+      </c>
+      <c r="C20" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.891416072845459</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7.63775</v>
+      </c>
+      <c r="H20" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.992241144180298</v>
+      </c>
+      <c r="B21" t="n">
+        <v>4.06256</v>
+      </c>
+      <c r="C21" t="n">
+        <v>10</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1.992854833602905</v>
+      </c>
+      <c r="G21" t="n">
+        <v>7.64503</v>
+      </c>
+      <c r="H21" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2.103638172149658</v>
+      </c>
+      <c r="B22" t="n">
+        <v>4.05528</v>
+      </c>
+      <c r="C22" t="n">
+        <v>10</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2.097615957260132</v>
+      </c>
+      <c r="G22" t="n">
+        <v>7.65594</v>
+      </c>
+      <c r="H22" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2.206740140914917</v>
+      </c>
+      <c r="B23" t="n">
+        <v>4.05892</v>
+      </c>
+      <c r="C23" t="n">
+        <v>10</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2.211894989013672</v>
+      </c>
+      <c r="G23" t="n">
+        <v>7.6523</v>
+      </c>
+      <c r="H23" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2.308221101760864</v>
+      </c>
+      <c r="B24" t="n">
+        <v>4.05528</v>
+      </c>
+      <c r="C24" t="n">
+        <v>10</v>
+      </c>
+      <c r="F24" t="n">
+        <v>2.308557033538818</v>
+      </c>
+      <c r="G24" t="n">
+        <v>7.6523</v>
+      </c>
+      <c r="H24" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.418142080307007</v>
+      </c>
+      <c r="B25" t="n">
+        <v>4.05528</v>
+      </c>
+      <c r="C25" t="n">
+        <v>10</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2.411791086196899</v>
+      </c>
+      <c r="G25" t="n">
+        <v>7.64866</v>
+      </c>
+      <c r="H25" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2.521491050720215</v>
+      </c>
+      <c r="B26" t="n">
+        <v>4.05892</v>
+      </c>
+      <c r="C26" t="n">
+        <v>10</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2.525809764862061</v>
+      </c>
+      <c r="G26" t="n">
+        <v>7.64503</v>
+      </c>
+      <c r="H26" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.623118162155151</v>
+      </c>
+      <c r="B27" t="n">
+        <v>4.04437</v>
+      </c>
+      <c r="C27" t="n">
+        <v>10</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2.62909197807312</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7.64866</v>
+      </c>
+      <c r="H27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.728261232376099</v>
+      </c>
+      <c r="B28" t="n">
+        <v>4.02982</v>
+      </c>
+      <c r="C28" t="n">
+        <v>10</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2.720979928970337</v>
+      </c>
+      <c r="G28" t="n">
+        <v>7.64139</v>
+      </c>
+      <c r="H28" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.836655139923096</v>
+      </c>
+      <c r="B29" t="n">
+        <v>4.01891</v>
+      </c>
+      <c r="C29" t="n">
+        <v>10</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2.839812994003296</v>
+      </c>
+      <c r="G29" t="n">
+        <v>7.64139</v>
+      </c>
+      <c r="H29" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2.939176082611084</v>
+      </c>
+      <c r="B30" t="n">
+        <v>4.02982</v>
+      </c>
+      <c r="C30" t="n">
+        <v>10</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2.945688009262085</v>
+      </c>
+      <c r="G30" t="n">
+        <v>7.63411</v>
+      </c>
+      <c r="H30" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3.044315338134766</v>
+      </c>
+      <c r="B31" t="n">
+        <v>4.02982</v>
+      </c>
+      <c r="C31" t="n">
+        <v>10</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3.046045780181885</v>
+      </c>
+      <c r="G31" t="n">
+        <v>7.6232</v>
+      </c>
+      <c r="H31" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>3.153427124023438</v>
+      </c>
+      <c r="B32" t="n">
+        <v>4.0371</v>
+      </c>
+      <c r="C32" t="n">
+        <v>10</v>
+      </c>
+      <c r="F32" t="n">
+        <v>3.145612955093384</v>
+      </c>
+      <c r="G32" t="n">
+        <v>7.61957</v>
+      </c>
+      <c r="H32" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>3.254815101623535</v>
+      </c>
+      <c r="B33" t="n">
+        <v>4.02982</v>
+      </c>
+      <c r="C33" t="n">
+        <v>10</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3.259254932403564</v>
+      </c>
+      <c r="G33" t="n">
+        <v>7.61593</v>
+      </c>
+      <c r="H33" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>3.357840299606323</v>
+      </c>
+      <c r="B34" t="n">
+        <v>4.03346</v>
+      </c>
+      <c r="C34" t="n">
+        <v>10</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3.362093925476074</v>
+      </c>
+      <c r="G34" t="n">
+        <v>7.62684</v>
+      </c>
+      <c r="H34" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>3.467922210693359</v>
+      </c>
+      <c r="B35" t="n">
+        <v>4.03346</v>
+      </c>
+      <c r="C35" t="n">
+        <v>10</v>
+      </c>
+      <c r="F35" t="n">
+        <v>3.464632987976074</v>
+      </c>
+      <c r="G35" t="n">
+        <v>7.63775</v>
+      </c>
+      <c r="H35" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>3.57062816619873</v>
+      </c>
+      <c r="B36" t="n">
+        <v>4.0371</v>
+      </c>
+      <c r="C36" t="n">
+        <v>10</v>
+      </c>
+      <c r="F36" t="n">
+        <v>3.574879884719849</v>
+      </c>
+      <c r="G36" t="n">
+        <v>7.64139</v>
+      </c>
+      <c r="H36" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>3.674376964569092</v>
+      </c>
+      <c r="B37" t="n">
+        <v>4.04073</v>
+      </c>
+      <c r="C37" t="n">
+        <v>10</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3.677172899246216</v>
+      </c>
+      <c r="G37" t="n">
+        <v>7.64866</v>
+      </c>
+      <c r="H37" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>3.775942325592041</v>
+      </c>
+      <c r="B38" t="n">
+        <v>4.04437</v>
+      </c>
+      <c r="C38" t="n">
+        <v>10</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3.780869960784912</v>
+      </c>
+      <c r="G38" t="n">
+        <v>7.66321</v>
+      </c>
+      <c r="H38" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>3.886831283569336</v>
+      </c>
+      <c r="B39" t="n">
+        <v>4.05165</v>
+      </c>
+      <c r="C39" t="n">
+        <v>10</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3.882690906524658</v>
+      </c>
+      <c r="G39" t="n">
+        <v>7.6523</v>
+      </c>
+      <c r="H39" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>3.988947153091431</v>
+      </c>
+      <c r="B40" t="n">
+        <v>4.04437</v>
+      </c>
+      <c r="C40" t="n">
+        <v>10</v>
+      </c>
+      <c r="F40" t="n">
+        <v>3.9933180809021</v>
+      </c>
+      <c r="G40" t="n">
+        <v>7.63775</v>
+      </c>
+      <c r="H40" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>4.091598272323608</v>
+      </c>
+      <c r="B41" t="n">
+        <v>4.03346</v>
+      </c>
+      <c r="C41" t="n">
+        <v>10</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4.095962047576904</v>
+      </c>
+      <c r="G41" t="n">
+        <v>7.64866</v>
+      </c>
+      <c r="H41" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>4.202208042144775</v>
+      </c>
+      <c r="B42" t="n">
+        <v>4.02255</v>
+      </c>
+      <c r="C42" t="n">
+        <v>10</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4.199067115783691</v>
+      </c>
+      <c r="G42" t="n">
+        <v>7.64866</v>
+      </c>
+      <c r="H42" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>4.305608987808228</v>
+      </c>
+      <c r="B43" t="n">
+        <v>4.01164</v>
+      </c>
+      <c r="C43" t="n">
+        <v>10</v>
+      </c>
+      <c r="F43" t="n">
+        <v>4.310024976730347</v>
+      </c>
+      <c r="G43" t="n">
+        <v>7.6523</v>
+      </c>
+      <c r="H43" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>4.407188177108765</v>
+      </c>
+      <c r="B44" t="n">
+        <v>4.008</v>
+      </c>
+      <c r="C44" t="n">
+        <v>10</v>
+      </c>
+      <c r="F44" t="n">
+        <v>4.412615776062012</v>
+      </c>
+      <c r="G44" t="n">
+        <v>7.66685</v>
+      </c>
+      <c r="H44" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>4.509643077850342</v>
+      </c>
+      <c r="B45" t="n">
+        <v>4.00436</v>
+      </c>
+      <c r="C45" t="n">
+        <v>10</v>
+      </c>
+      <c r="F45" t="n">
+        <v>4.515186786651611</v>
+      </c>
+      <c r="G45" t="n">
+        <v>7.6814</v>
+      </c>
+      <c r="H45" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>4.620038270950317</v>
+      </c>
+      <c r="B46" t="n">
+        <v>4.00073</v>
+      </c>
+      <c r="C46" t="n">
+        <v>10</v>
+      </c>
+      <c r="F46" t="n">
+        <v>4.617035865783691</v>
+      </c>
+      <c r="G46" t="n">
+        <v>7.68503</v>
+      </c>
+      <c r="H46" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>4.722289323806763</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3.99345</v>
+      </c>
+      <c r="C47" t="n">
+        <v>10</v>
+      </c>
+      <c r="F47" t="n">
+        <v>4.728153944015503</v>
+      </c>
+      <c r="G47" t="n">
+        <v>7.67412</v>
+      </c>
+      <c r="H47" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>4.826080083847046</v>
+      </c>
+      <c r="B48" t="n">
+        <v>3.98254</v>
+      </c>
+      <c r="C48" t="n">
+        <v>10</v>
+      </c>
+      <c r="F48" t="n">
+        <v>4.830190896987915</v>
+      </c>
+      <c r="G48" t="n">
+        <v>7.66321</v>
+      </c>
+      <c r="H48" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>4.938929319381714</v>
+      </c>
+      <c r="B49" t="n">
+        <v>3.97527</v>
+      </c>
+      <c r="C49" t="n">
+        <v>10</v>
+      </c>
+      <c r="F49" t="n">
+        <v>4.931764841079712</v>
+      </c>
+      <c r="G49" t="n">
+        <v>7.65957</v>
+      </c>
+      <c r="H49" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>5.038088083267212</v>
+      </c>
+      <c r="B50" t="n">
+        <v>3.96436</v>
+      </c>
+      <c r="C50" t="n">
+        <v>10</v>
+      </c>
+      <c r="F50" t="n">
+        <v>5.042779922485352</v>
+      </c>
+      <c r="G50" t="n">
+        <v>7.65957</v>
+      </c>
+      <c r="H50" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:S50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Throttle</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Throttle</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>Throttle</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="Q1" s="3" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="R1" s="3" t="inlineStr">
+        <is>
+          <t>Throttle</t>
+        </is>
+      </c>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>9.5367431640625e-07</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3.56065</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGE(B$2:B$10000)</f>
+        <v/>
+      </c>
+      <c r="F2" t="n">
+        <v>9.5367431640625e-07</v>
+      </c>
+      <c r="G2" t="n">
+        <v>7.49227</v>
+      </c>
+      <c r="H2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(G$2:G$10000)</f>
+        <v/>
+      </c>
+      <c r="K2" t="n">
+        <v>9.5367431640625e-07</v>
+      </c>
+      <c r="L2" t="n">
+        <v>10.8347</v>
+      </c>
+      <c r="M2" t="n">
+        <v>30</v>
+      </c>
+      <c r="N2">
+        <f>AVERAGE(L$2:L$10000)</f>
+        <v/>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>14.44626</v>
+      </c>
+      <c r="R2" t="n">
+        <v>40</v>
+      </c>
+      <c r="S2">
+        <f>AVERAGE(Q$2:Q$10000)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0.107313871383667</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3.57883</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.1066551208496094</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7.51046</v>
+      </c>
+      <c r="H3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.1033759117126465</v>
+      </c>
+      <c r="L3" t="n">
+        <v>10.84561</v>
+      </c>
+      <c r="M3" t="n">
+        <v>30</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.1190941333770752</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>14.4499</v>
+      </c>
+      <c r="R3" t="n">
+        <v>40</v>
+      </c>
+      <c r="S3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.2171146869659424</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3.59702</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.2083489894866943</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7.52864</v>
+      </c>
+      <c r="H4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.2051188945770264</v>
+      </c>
+      <c r="L4" t="n">
+        <v>10.83833</v>
+      </c>
+      <c r="M4" t="n">
+        <v>30</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.2190821170806885</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>14.45717</v>
+      </c>
+      <c r="R4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.3196616172790527</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.60793</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.3187520503997803</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7.53591</v>
+      </c>
+      <c r="H5" t="n">
+        <v>20</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.3197319507598877</v>
+      </c>
+      <c r="L5" t="n">
+        <v>10.8347</v>
+      </c>
+      <c r="M5" t="n">
+        <v>30</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.3207371234893799</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>14.45354</v>
+      </c>
+      <c r="R5" t="n">
+        <v>40</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.4228389263153076</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3.60065</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.4223439693450928</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7.53955</v>
+      </c>
+      <c r="H6" t="n">
+        <v>20</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.422680139541626</v>
+      </c>
+      <c r="L6" t="n">
+        <v>10.83106</v>
+      </c>
+      <c r="M6" t="n">
+        <v>30</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.4360520839691162</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>14.44626</v>
+      </c>
+      <c r="R6" t="n">
+        <v>40</v>
+      </c>
+      <c r="S6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.5265789031982422</v>
+      </c>
+      <c r="B7" t="n">
+        <v>3.59702</v>
+      </c>
+      <c r="C7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.5255420207977295</v>
+      </c>
+      <c r="G7" t="n">
+        <v>7.53228</v>
+      </c>
+      <c r="H7" t="n">
+        <v>20</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.5224010944366455</v>
+      </c>
+      <c r="L7" t="n">
+        <v>10.82379</v>
+      </c>
+      <c r="M7" t="n">
+        <v>30</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.5385448932647705</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>14.44262</v>
+      </c>
+      <c r="R7" t="n">
+        <v>40</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.6350958347320557</v>
+      </c>
+      <c r="B8" t="n">
+        <v>3.60065</v>
+      </c>
+      <c r="C8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.6349210739135742</v>
+      </c>
+      <c r="G8" t="n">
+        <v>7.525</v>
+      </c>
+      <c r="H8" t="n">
+        <v>20</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.6355369091033936</v>
+      </c>
+      <c r="L8" t="n">
+        <v>10.81651</v>
+      </c>
+      <c r="M8" t="n">
+        <v>30</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.6414260864257812</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>14.44626</v>
+      </c>
+      <c r="R8" t="n">
+        <v>40</v>
+      </c>
+      <c r="S8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.7382748126983643</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3.59702</v>
+      </c>
+      <c r="C9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.7391469478607178</v>
+      </c>
+      <c r="G9" t="n">
+        <v>7.52864</v>
+      </c>
+      <c r="H9" t="n">
+        <v>20</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.7380669116973877</v>
+      </c>
+      <c r="L9" t="n">
+        <v>10.81651</v>
+      </c>
+      <c r="M9" t="n">
+        <v>30</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.7508618831634521</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>14.4499</v>
+      </c>
+      <c r="R9" t="n">
+        <v>40</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.8422868251800537</v>
+      </c>
+      <c r="B10" t="n">
+        <v>3.59702</v>
+      </c>
+      <c r="C10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.8414969444274902</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7.525</v>
+      </c>
+      <c r="H10" t="n">
+        <v>20</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.8395318984985352</v>
+      </c>
+      <c r="L10" t="n">
+        <v>10.80196</v>
+      </c>
+      <c r="M10" t="n">
+        <v>30</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.8532428741455078</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>14.45354</v>
+      </c>
+      <c r="R10" t="n">
+        <v>40</v>
+      </c>
+      <c r="S10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.9526529312133789</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3.58247</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9504439830780029</v>
+      </c>
+      <c r="G11" t="n">
+        <v>7.525</v>
+      </c>
+      <c r="H11" t="n">
+        <v>20</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.9511709213256836</v>
+      </c>
+      <c r="L11" t="n">
+        <v>10.78742</v>
+      </c>
+      <c r="M11" t="n">
+        <v>30</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.9567549228668213</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>14.46081</v>
+      </c>
+      <c r="R11" t="n">
+        <v>40</v>
+      </c>
+      <c r="S11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.055234670639038</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3.56428</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.053596019744873</v>
+      </c>
+      <c r="G12" t="n">
+        <v>7.53591</v>
+      </c>
+      <c r="H12" t="n">
+        <v>20</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1.053250074386597</v>
+      </c>
+      <c r="L12" t="n">
+        <v>10.77287</v>
+      </c>
+      <c r="M12" t="n">
+        <v>30</v>
+      </c>
+      <c r="P12" t="n">
+        <v>1.057636022567749</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>14.45354</v>
+      </c>
+      <c r="R12" t="n">
+        <v>40</v>
+      </c>
+      <c r="S12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1.157279968261719</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3.54974</v>
+      </c>
+      <c r="C13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.1581130027771</v>
+      </c>
+      <c r="G13" t="n">
+        <v>7.54319</v>
+      </c>
+      <c r="H13" t="n">
+        <v>20</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.15546703338623</v>
+      </c>
+      <c r="L13" t="n">
+        <v>10.76196</v>
+      </c>
+      <c r="M13" t="n">
+        <v>30</v>
+      </c>
+      <c r="P13" t="n">
+        <v>1.170032024383545</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>14.45354</v>
+      </c>
+      <c r="R13" t="n">
+        <v>40</v>
+      </c>
+      <c r="S13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.267973661422729</v>
+      </c>
+      <c r="B14" t="n">
+        <v>3.5461</v>
+      </c>
+      <c r="C14" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.259054899215698</v>
+      </c>
+      <c r="G14" t="n">
+        <v>7.54683</v>
+      </c>
+      <c r="H14" t="n">
+        <v>20</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1.259373903274536</v>
+      </c>
+      <c r="L14" t="n">
+        <v>10.75832</v>
+      </c>
+      <c r="M14" t="n">
+        <v>30</v>
+      </c>
+      <c r="P14" t="n">
+        <v>1.27276611328125</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>14.44626</v>
+      </c>
+      <c r="R14" t="n">
+        <v>40</v>
+      </c>
+      <c r="S14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.370136022567749</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3.5461</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.368195772171021</v>
+      </c>
+      <c r="G15" t="n">
+        <v>7.5541</v>
+      </c>
+      <c r="H15" t="n">
+        <v>20</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1.368654727935791</v>
+      </c>
+      <c r="L15" t="n">
+        <v>10.75104</v>
+      </c>
+      <c r="M15" t="n">
+        <v>30</v>
+      </c>
+      <c r="P15" t="n">
+        <v>1.374266862869263</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>14.4499</v>
+      </c>
+      <c r="R15" t="n">
+        <v>40</v>
+      </c>
+      <c r="S15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.471787929534912</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3.5461</v>
+      </c>
+      <c r="C16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.471979141235352</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7.55774</v>
+      </c>
+      <c r="H16" t="n">
+        <v>20</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.473219156265259</v>
+      </c>
+      <c r="L16" t="n">
+        <v>10.74013</v>
+      </c>
+      <c r="M16" t="n">
+        <v>30</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1.484179973602295</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>14.46808</v>
+      </c>
+      <c r="R16" t="n">
+        <v>40</v>
+      </c>
+      <c r="S16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.583256006240845</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3.54974</v>
+      </c>
+      <c r="C17" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.573632001876831</v>
+      </c>
+      <c r="G17" t="n">
+        <v>7.54683</v>
+      </c>
+      <c r="H17" t="n">
+        <v>20</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1.574802875518799</v>
+      </c>
+      <c r="L17" t="n">
+        <v>10.72922</v>
+      </c>
+      <c r="M17" t="n">
+        <v>30</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1.586948871612549</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>14.48991</v>
+      </c>
+      <c r="R17" t="n">
+        <v>40</v>
+      </c>
+      <c r="S17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.685508728027344</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3.53155</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.685081958770752</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7.53591</v>
+      </c>
+      <c r="H18" t="n">
+        <v>20</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1.685268878936768</v>
+      </c>
+      <c r="L18" t="n">
+        <v>10.72195</v>
+      </c>
+      <c r="M18" t="n">
+        <v>30</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1.690385103225708</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>14.50809</v>
+      </c>
+      <c r="R18" t="n">
+        <v>40</v>
+      </c>
+      <c r="S18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.78871488571167</v>
+      </c>
+      <c r="B19" t="n">
+        <v>3.51337</v>
+      </c>
+      <c r="C19" t="n">
+        <v>10</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.788208961486816</v>
+      </c>
+      <c r="G19" t="n">
+        <v>7.52864</v>
+      </c>
+      <c r="H19" t="n">
+        <v>20</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1.787741899490356</v>
+      </c>
+      <c r="L19" t="n">
+        <v>10.71831</v>
+      </c>
+      <c r="M19" t="n">
+        <v>30</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1.800075054168701</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>14.51173</v>
+      </c>
+      <c r="R19" t="n">
+        <v>40</v>
+      </c>
+      <c r="S19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.889122724533081</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3.50245</v>
+      </c>
+      <c r="C20" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.890118837356567</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7.51773</v>
+      </c>
+      <c r="H20" t="n">
+        <v>20</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1.891273021697998</v>
+      </c>
+      <c r="L20" t="n">
+        <v>10.70376</v>
+      </c>
+      <c r="M20" t="n">
+        <v>30</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1.90558385848999</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>14.50809</v>
+      </c>
+      <c r="R20" t="n">
+        <v>40</v>
+      </c>
+      <c r="S20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.996445894241333</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3.48791</v>
+      </c>
+      <c r="C21" t="n">
+        <v>10</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2.000174999237061</v>
+      </c>
+      <c r="G21" t="n">
+        <v>7.51046</v>
+      </c>
+      <c r="H21" t="n">
+        <v>20</v>
+      </c>
+      <c r="K21" t="n">
+        <v>2.001492023468018</v>
+      </c>
+      <c r="L21" t="n">
+        <v>10.69285</v>
+      </c>
+      <c r="M21" t="n">
+        <v>30</v>
+      </c>
+      <c r="P21" t="n">
+        <v>2.005390882492065</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>14.51173</v>
+      </c>
+      <c r="R21" t="n">
+        <v>40</v>
+      </c>
+      <c r="S21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2.1021409034729</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.47336</v>
+      </c>
+      <c r="C22" t="n">
+        <v>10</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2.102818965911865</v>
+      </c>
+      <c r="G22" t="n">
+        <v>7.50318</v>
+      </c>
+      <c r="H22" t="n">
+        <v>20</v>
+      </c>
+      <c r="K22" t="n">
+        <v>2.104347944259644</v>
+      </c>
+      <c r="L22" t="n">
+        <v>10.68194</v>
+      </c>
+      <c r="M22" t="n">
+        <v>30</v>
+      </c>
+      <c r="P22" t="n">
+        <v>2.107569932937622</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>14.50445</v>
+      </c>
+      <c r="R22" t="n">
+        <v>40</v>
+      </c>
+      <c r="S22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2.207225799560547</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.46245</v>
+      </c>
+      <c r="C23" t="n">
+        <v>10</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2.20566987991333</v>
+      </c>
+      <c r="G23" t="n">
+        <v>7.50318</v>
+      </c>
+      <c r="H23" t="n">
+        <v>20</v>
+      </c>
+      <c r="K23" t="n">
+        <v>2.204864978790283</v>
+      </c>
+      <c r="L23" t="n">
+        <v>10.67103</v>
+      </c>
+      <c r="M23" t="n">
+        <v>30</v>
+      </c>
+      <c r="P23" t="n">
+        <v>2.218262195587158</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>14.50809</v>
+      </c>
+      <c r="R23" t="n">
+        <v>40</v>
+      </c>
+      <c r="S23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2.317654848098755</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3.45881</v>
+      </c>
+      <c r="C24" t="n">
+        <v>10</v>
+      </c>
+      <c r="F24" t="n">
+        <v>2.321324110031128</v>
+      </c>
+      <c r="G24" t="n">
+        <v>7.51409</v>
+      </c>
+      <c r="H24" t="n">
+        <v>20</v>
+      </c>
+      <c r="K24" t="n">
+        <v>2.316529989242554</v>
+      </c>
+      <c r="L24" t="n">
+        <v>10.66739</v>
+      </c>
+      <c r="M24" t="n">
+        <v>30</v>
+      </c>
+      <c r="P24" t="n">
+        <v>2.320533037185669</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>14.52628</v>
+      </c>
+      <c r="R24" t="n">
+        <v>40</v>
+      </c>
+      <c r="S24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.41973876953125</v>
+      </c>
+      <c r="B25" t="n">
+        <v>3.4479</v>
+      </c>
+      <c r="C25" t="n">
+        <v>10</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2.419510126113892</v>
+      </c>
+      <c r="G25" t="n">
+        <v>7.525</v>
+      </c>
+      <c r="H25" t="n">
+        <v>20</v>
+      </c>
+      <c r="K25" t="n">
+        <v>2.419832706451416</v>
+      </c>
+      <c r="L25" t="n">
+        <v>10.66376</v>
+      </c>
+      <c r="M25" t="n">
+        <v>30</v>
+      </c>
+      <c r="P25" t="n">
+        <v>2.425064086914062</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>14.52991</v>
+      </c>
+      <c r="R25" t="n">
+        <v>40</v>
+      </c>
+      <c r="S25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2.522672891616821</v>
+      </c>
+      <c r="B26" t="n">
+        <v>3.4479</v>
+      </c>
+      <c r="C26" t="n">
+        <v>10</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2.522324085235596</v>
+      </c>
+      <c r="G26" t="n">
+        <v>7.53955</v>
+      </c>
+      <c r="H26" t="n">
+        <v>20</v>
+      </c>
+      <c r="K26" t="n">
+        <v>2.520380973815918</v>
+      </c>
+      <c r="L26" t="n">
+        <v>10.66012</v>
+      </c>
+      <c r="M26" t="n">
+        <v>30</v>
+      </c>
+      <c r="P26" t="n">
+        <v>2.533601045608521</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>14.5481</v>
+      </c>
+      <c r="R26" t="n">
+        <v>40</v>
+      </c>
+      <c r="S26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.636922836303711</v>
+      </c>
+      <c r="B27" t="n">
+        <v>3.44426</v>
+      </c>
+      <c r="C27" t="n">
+        <v>10</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2.626193046569824</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7.53228</v>
+      </c>
+      <c r="H27" t="n">
+        <v>20</v>
+      </c>
+      <c r="K27" t="n">
+        <v>2.624588966369629</v>
+      </c>
+      <c r="L27" t="n">
+        <v>10.66012</v>
+      </c>
+      <c r="M27" t="n">
+        <v>30</v>
+      </c>
+      <c r="P27" t="n">
+        <v>2.638822078704834</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>14.56628</v>
+      </c>
+      <c r="R27" t="n">
+        <v>40</v>
+      </c>
+      <c r="S27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.734553813934326</v>
+      </c>
+      <c r="B28" t="n">
+        <v>3.45881</v>
+      </c>
+      <c r="C28" t="n">
+        <v>10</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2.740495920181274</v>
+      </c>
+      <c r="G28" t="n">
+        <v>7.52137</v>
+      </c>
+      <c r="H28" t="n">
+        <v>20</v>
+      </c>
+      <c r="K28" t="n">
+        <v>2.73432183265686</v>
+      </c>
+      <c r="L28" t="n">
+        <v>10.66739</v>
+      </c>
+      <c r="M28" t="n">
+        <v>30</v>
+      </c>
+      <c r="P28" t="n">
+        <v>2.740933895111084</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>14.58447</v>
+      </c>
+      <c r="R28" t="n">
+        <v>40</v>
+      </c>
+      <c r="S28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.83758282661438</v>
+      </c>
+      <c r="B29" t="n">
+        <v>3.46972</v>
+      </c>
+      <c r="C29" t="n">
+        <v>10</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2.837402820587158</v>
+      </c>
+      <c r="G29" t="n">
+        <v>7.50682</v>
+      </c>
+      <c r="H29" t="n">
+        <v>20</v>
+      </c>
+      <c r="K29" t="n">
+        <v>2.836881875991821</v>
+      </c>
+      <c r="L29" t="n">
+        <v>10.67103</v>
+      </c>
+      <c r="M29" t="n">
+        <v>30</v>
+      </c>
+      <c r="P29" t="n">
+        <v>2.855487108230591</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>14.58447</v>
+      </c>
+      <c r="R29" t="n">
+        <v>40</v>
+      </c>
+      <c r="S29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2.952573776245117</v>
+      </c>
+      <c r="B30" t="n">
+        <v>3.47336</v>
+      </c>
+      <c r="C30" t="n">
+        <v>10</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2.939684867858887</v>
+      </c>
+      <c r="G30" t="n">
+        <v>7.49591</v>
+      </c>
+      <c r="H30" t="n">
+        <v>20</v>
+      </c>
+      <c r="K30" t="n">
+        <v>2.939452886581421</v>
+      </c>
+      <c r="L30" t="n">
+        <v>10.67467</v>
+      </c>
+      <c r="M30" t="n">
+        <v>30</v>
+      </c>
+      <c r="P30" t="n">
+        <v>2.953548192977905</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>14.58447</v>
+      </c>
+      <c r="R30" t="n">
+        <v>40</v>
+      </c>
+      <c r="S30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3.056894779205322</v>
+      </c>
+      <c r="B31" t="n">
+        <v>3.47336</v>
+      </c>
+      <c r="C31" t="n">
+        <v>10</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3.049037933349609</v>
+      </c>
+      <c r="G31" t="n">
+        <v>7.49591</v>
+      </c>
+      <c r="H31" t="n">
+        <v>20</v>
+      </c>
+      <c r="K31" t="n">
+        <v>3.054257869720459</v>
+      </c>
+      <c r="L31" t="n">
+        <v>10.68194</v>
+      </c>
+      <c r="M31" t="n">
+        <v>30</v>
+      </c>
+      <c r="P31" t="n">
+        <v>3.054487943649292</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>14.58811</v>
+      </c>
+      <c r="R31" t="n">
+        <v>40</v>
+      </c>
+      <c r="S31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>3.153355836868286</v>
+      </c>
+      <c r="B32" t="n">
+        <v>3.46972</v>
+      </c>
+      <c r="C32" t="n">
+        <v>10</v>
+      </c>
+      <c r="F32" t="n">
+        <v>3.15467095375061</v>
+      </c>
+      <c r="G32" t="n">
+        <v>7.48863</v>
+      </c>
+      <c r="H32" t="n">
+        <v>20</v>
+      </c>
+      <c r="K32" t="n">
+        <v>3.156433820724487</v>
+      </c>
+      <c r="L32" t="n">
+        <v>10.68194</v>
+      </c>
+      <c r="M32" t="n">
+        <v>30</v>
+      </c>
+      <c r="P32" t="n">
+        <v>3.156583070755005</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>14.60265</v>
+      </c>
+      <c r="R32" t="n">
+        <v>40</v>
+      </c>
+      <c r="S32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>3.255394697189331</v>
+      </c>
+      <c r="B33" t="n">
+        <v>3.46245</v>
+      </c>
+      <c r="C33" t="n">
+        <v>10</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3.255593061447144</v>
+      </c>
+      <c r="G33" t="n">
+        <v>7.46681</v>
+      </c>
+      <c r="H33" t="n">
+        <v>20</v>
+      </c>
+      <c r="K33" t="n">
+        <v>3.255744934082031</v>
+      </c>
+      <c r="L33" t="n">
+        <v>10.69649</v>
+      </c>
+      <c r="M33" t="n">
+        <v>30</v>
+      </c>
+      <c r="P33" t="n">
+        <v>3.270409107208252</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>14.59902</v>
+      </c>
+      <c r="R33" t="n">
+        <v>40</v>
+      </c>
+      <c r="S33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>3.371399879455566</v>
+      </c>
+      <c r="B34" t="n">
+        <v>3.46608</v>
+      </c>
+      <c r="C34" t="n">
+        <v>10</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3.370265960693359</v>
+      </c>
+      <c r="G34" t="n">
+        <v>7.45954</v>
+      </c>
+      <c r="H34" t="n">
+        <v>20</v>
+      </c>
+      <c r="K34" t="n">
+        <v>3.369927883148193</v>
+      </c>
+      <c r="L34" t="n">
+        <v>10.70376</v>
+      </c>
+      <c r="M34" t="n">
+        <v>30</v>
+      </c>
+      <c r="P34" t="n">
+        <v>3.368242025375366</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>14.59174</v>
+      </c>
+      <c r="R34" t="n">
+        <v>40</v>
+      </c>
+      <c r="S34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>3.473310947418213</v>
+      </c>
+      <c r="B35" t="n">
+        <v>3.46972</v>
+      </c>
+      <c r="C35" t="n">
+        <v>10</v>
+      </c>
+      <c r="F35" t="n">
+        <v>3.471826076507568</v>
+      </c>
+      <c r="G35" t="n">
+        <v>7.46317</v>
+      </c>
+      <c r="H35" t="n">
+        <v>20</v>
+      </c>
+      <c r="K35" t="n">
+        <v>3.472630977630615</v>
+      </c>
+      <c r="L35" t="n">
+        <v>10.70013</v>
+      </c>
+      <c r="M35" t="n">
+        <v>30</v>
+      </c>
+      <c r="P35" t="n">
+        <v>3.474420070648193</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>14.57719</v>
+      </c>
+      <c r="R35" t="n">
+        <v>40</v>
+      </c>
+      <c r="S35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>3.572480916976929</v>
+      </c>
+      <c r="B36" t="n">
+        <v>3.48427</v>
+      </c>
+      <c r="C36" t="n">
+        <v>10</v>
+      </c>
+      <c r="F36" t="n">
+        <v>3.576740980148315</v>
+      </c>
+      <c r="G36" t="n">
+        <v>7.46681</v>
+      </c>
+      <c r="H36" t="n">
+        <v>20</v>
+      </c>
+      <c r="K36" t="n">
+        <v>3.57491397857666</v>
+      </c>
+      <c r="L36" t="n">
+        <v>10.70013</v>
+      </c>
+      <c r="M36" t="n">
+        <v>30</v>
+      </c>
+      <c r="P36" t="n">
+        <v>3.587707042694092</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>14.57356</v>
+      </c>
+      <c r="R36" t="n">
+        <v>40</v>
+      </c>
+      <c r="S36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>3.6871018409729</v>
+      </c>
+      <c r="B37" t="n">
+        <v>3.48791</v>
+      </c>
+      <c r="C37" t="n">
+        <v>10</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3.684927940368652</v>
+      </c>
+      <c r="G37" t="n">
+        <v>7.46681</v>
+      </c>
+      <c r="H37" t="n">
+        <v>20</v>
+      </c>
+      <c r="K37" t="n">
+        <v>3.672811031341553</v>
+      </c>
+      <c r="L37" t="n">
+        <v>10.69285</v>
+      </c>
+      <c r="M37" t="n">
+        <v>30</v>
+      </c>
+      <c r="P37" t="n">
+        <v>3.68989086151123</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>14.57356</v>
+      </c>
+      <c r="R37" t="n">
+        <v>40</v>
+      </c>
+      <c r="S37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>3.790974855422974</v>
+      </c>
+      <c r="B38" t="n">
+        <v>3.48791</v>
+      </c>
+      <c r="C38" t="n">
+        <v>10</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3.788552045822144</v>
+      </c>
+      <c r="G38" t="n">
+        <v>7.45954</v>
+      </c>
+      <c r="H38" t="n">
+        <v>20</v>
+      </c>
+      <c r="K38" t="n">
+        <v>3.788054943084717</v>
+      </c>
+      <c r="L38" t="n">
+        <v>10.68558</v>
+      </c>
+      <c r="M38" t="n">
+        <v>30</v>
+      </c>
+      <c r="P38" t="n">
+        <v>3.794732093811035</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>14.58083</v>
+      </c>
+      <c r="R38" t="n">
+        <v>40</v>
+      </c>
+      <c r="S38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>3.891268730163574</v>
+      </c>
+      <c r="B39" t="n">
+        <v>3.48791</v>
+      </c>
+      <c r="C39" t="n">
+        <v>10</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3.89067816734314</v>
+      </c>
+      <c r="G39" t="n">
+        <v>7.46317</v>
+      </c>
+      <c r="H39" t="n">
+        <v>20</v>
+      </c>
+      <c r="K39" t="n">
+        <v>3.890222787857056</v>
+      </c>
+      <c r="L39" t="n">
+        <v>10.68194</v>
+      </c>
+      <c r="M39" t="n">
+        <v>30</v>
+      </c>
+      <c r="P39" t="n">
+        <v>3.903708934783936</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>14.57719</v>
+      </c>
+      <c r="R39" t="n">
+        <v>40</v>
+      </c>
+      <c r="S39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>4.001823902130127</v>
+      </c>
+      <c r="B40" t="n">
+        <v>3.50609</v>
+      </c>
+      <c r="C40" t="n">
+        <v>10</v>
+      </c>
+      <c r="F40" t="n">
+        <v>3.994566917419434</v>
+      </c>
+      <c r="G40" t="n">
+        <v>7.4559</v>
+      </c>
+      <c r="H40" t="n">
+        <v>20</v>
+      </c>
+      <c r="K40" t="n">
+        <v>3.987718820571899</v>
+      </c>
+      <c r="L40" t="n">
+        <v>10.68194</v>
+      </c>
+      <c r="M40" t="n">
+        <v>30</v>
+      </c>
+      <c r="P40" t="n">
+        <v>4.007064819335938</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>14.57719</v>
+      </c>
+      <c r="R40" t="n">
+        <v>40</v>
+      </c>
+      <c r="S40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>4.105463743209839</v>
+      </c>
+      <c r="B41" t="n">
+        <v>3.52064</v>
+      </c>
+      <c r="C41" t="n">
+        <v>10</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4.103394031524658</v>
+      </c>
+      <c r="G41" t="n">
+        <v>7.43772</v>
+      </c>
+      <c r="H41" t="n">
+        <v>20</v>
+      </c>
+      <c r="K41" t="n">
+        <v>4.102702856063843</v>
+      </c>
+      <c r="L41" t="n">
+        <v>10.68194</v>
+      </c>
+      <c r="M41" t="n">
+        <v>30</v>
+      </c>
+      <c r="P41" t="n">
+        <v>4.108866930007935</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>14.58083</v>
+      </c>
+      <c r="R41" t="n">
+        <v>40</v>
+      </c>
+      <c r="S41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>4.203877687454224</v>
+      </c>
+      <c r="B42" t="n">
+        <v>3.53155</v>
+      </c>
+      <c r="C42" t="n">
+        <v>10</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4.205923795700073</v>
+      </c>
+      <c r="G42" t="n">
+        <v>7.41589</v>
+      </c>
+      <c r="H42" t="n">
+        <v>20</v>
+      </c>
+      <c r="K42" t="n">
+        <v>4.206860065460205</v>
+      </c>
+      <c r="L42" t="n">
+        <v>10.67467</v>
+      </c>
+      <c r="M42" t="n">
+        <v>30</v>
+      </c>
+      <c r="P42" t="n">
+        <v>4.219772100448608</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>14.56992</v>
+      </c>
+      <c r="R42" t="n">
+        <v>40</v>
+      </c>
+      <c r="S42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>4.309773683547974</v>
+      </c>
+      <c r="B43" t="n">
+        <v>3.53519</v>
+      </c>
+      <c r="C43" t="n">
+        <v>10</v>
+      </c>
+      <c r="F43" t="n">
+        <v>4.308702945709229</v>
+      </c>
+      <c r="G43" t="n">
+        <v>7.40135</v>
+      </c>
+      <c r="H43" t="n">
+        <v>20</v>
+      </c>
+      <c r="K43" t="n">
+        <v>4.310493946075439</v>
+      </c>
+      <c r="L43" t="n">
+        <v>10.67467</v>
+      </c>
+      <c r="M43" t="n">
+        <v>30</v>
+      </c>
+      <c r="P43" t="n">
+        <v>4.32288122177124</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>14.55174</v>
+      </c>
+      <c r="R43" t="n">
+        <v>40</v>
+      </c>
+      <c r="S43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>4.421341896057129</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3.52428</v>
+      </c>
+      <c r="C44" t="n">
+        <v>10</v>
+      </c>
+      <c r="F44" t="n">
+        <v>4.419363975524902</v>
+      </c>
+      <c r="G44" t="n">
+        <v>7.3868</v>
+      </c>
+      <c r="H44" t="n">
+        <v>20</v>
+      </c>
+      <c r="K44" t="n">
+        <v>4.419242858886719</v>
+      </c>
+      <c r="L44" t="n">
+        <v>10.67467</v>
+      </c>
+      <c r="M44" t="n">
+        <v>30</v>
+      </c>
+      <c r="P44" t="n">
+        <v>4.425400972366333</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>14.52991</v>
+      </c>
+      <c r="R44" t="n">
+        <v>40</v>
+      </c>
+      <c r="S44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>4.524090766906738</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.52791</v>
+      </c>
+      <c r="C45" t="n">
+        <v>10</v>
+      </c>
+      <c r="F45" t="n">
+        <v>4.522217988967896</v>
+      </c>
+      <c r="G45" t="n">
+        <v>7.3868</v>
+      </c>
+      <c r="H45" t="n">
+        <v>20</v>
+      </c>
+      <c r="K45" t="n">
+        <v>4.521610021591187</v>
+      </c>
+      <c r="L45" t="n">
+        <v>10.66739</v>
+      </c>
+      <c r="M45" t="n">
+        <v>30</v>
+      </c>
+      <c r="P45" t="n">
+        <v>4.527545928955078</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>14.52264</v>
+      </c>
+      <c r="R45" t="n">
+        <v>40</v>
+      </c>
+      <c r="S45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>4.625074863433838</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3.52791</v>
+      </c>
+      <c r="C46" t="n">
+        <v>10</v>
+      </c>
+      <c r="F46" t="n">
+        <v>4.624560832977295</v>
+      </c>
+      <c r="G46" t="n">
+        <v>7.39771</v>
+      </c>
+      <c r="H46" t="n">
+        <v>20</v>
+      </c>
+      <c r="K46" t="n">
+        <v>4.62418794631958</v>
+      </c>
+      <c r="L46" t="n">
+        <v>10.66012</v>
+      </c>
+      <c r="M46" t="n">
+        <v>30</v>
+      </c>
+      <c r="P46" t="n">
+        <v>4.636475086212158</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>14.52264</v>
+      </c>
+      <c r="R46" t="n">
+        <v>40</v>
+      </c>
+      <c r="S46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>4.7372727394104</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3.52791</v>
+      </c>
+      <c r="C47" t="n">
+        <v>10</v>
+      </c>
+      <c r="F47" t="n">
+        <v>4.736140012741089</v>
+      </c>
+      <c r="G47" t="n">
+        <v>7.39407</v>
+      </c>
+      <c r="H47" t="n">
+        <v>20</v>
+      </c>
+      <c r="K47" t="n">
+        <v>4.726864814758301</v>
+      </c>
+      <c r="L47" t="n">
+        <v>10.66739</v>
+      </c>
+      <c r="M47" t="n">
+        <v>30</v>
+      </c>
+      <c r="P47" t="n">
+        <v>4.739576816558838</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>14.52628</v>
+      </c>
+      <c r="R47" t="n">
+        <v>40</v>
+      </c>
+      <c r="S47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>4.839401960372925</v>
+      </c>
+      <c r="B48" t="n">
+        <v>3.53883</v>
+      </c>
+      <c r="C48" t="n">
+        <v>10</v>
+      </c>
+      <c r="F48" t="n">
+        <v>4.838207006454468</v>
+      </c>
+      <c r="G48" t="n">
+        <v>7.38316</v>
+      </c>
+      <c r="H48" t="n">
+        <v>20</v>
+      </c>
+      <c r="K48" t="n">
+        <v>4.839567899703979</v>
+      </c>
+      <c r="L48" t="n">
+        <v>10.68194</v>
+      </c>
+      <c r="M48" t="n">
+        <v>30</v>
+      </c>
+      <c r="P48" t="n">
+        <v>4.841856002807617</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>14.52991</v>
+      </c>
+      <c r="R48" t="n">
+        <v>40</v>
+      </c>
+      <c r="S48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>4.941390752792358</v>
+      </c>
+      <c r="B49" t="n">
+        <v>3.54246</v>
+      </c>
+      <c r="C49" t="n">
+        <v>10</v>
+      </c>
+      <c r="F49" t="n">
+        <v>4.94209098815918</v>
+      </c>
+      <c r="G49" t="n">
+        <v>7.37589</v>
+      </c>
+      <c r="H49" t="n">
+        <v>20</v>
+      </c>
+      <c r="K49" t="n">
+        <v>4.94106388092041</v>
+      </c>
+      <c r="L49" t="n">
+        <v>10.68558</v>
+      </c>
+      <c r="M49" t="n">
+        <v>30</v>
+      </c>
+      <c r="P49" t="n">
+        <v>4.953572988510132</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>14.52991</v>
+      </c>
+      <c r="R49" t="n">
+        <v>40</v>
+      </c>
+      <c r="S49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>5.051864624023438</v>
+      </c>
+      <c r="B50" t="n">
+        <v>3.54246</v>
+      </c>
+      <c r="C50" t="n">
+        <v>10</v>
+      </c>
+      <c r="F50" t="n">
+        <v>5.050673961639404</v>
+      </c>
+      <c r="G50" t="n">
+        <v>7.37589</v>
+      </c>
+      <c r="H50" t="n">
+        <v>20</v>
+      </c>
+      <c r="K50" t="n">
+        <v>5.043577909469604</v>
+      </c>
+      <c r="L50" t="n">
+        <v>10.6783</v>
+      </c>
+      <c r="M50" t="n">
+        <v>30</v>
+      </c>
+      <c r="P50" t="n">
+        <v>5.049707174301147</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>14.52991</v>
+      </c>
+      <c r="R50" t="n">
+        <v>40</v>
+      </c>
+      <c r="S50" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added more precise sheet naming
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -35320,7 +35320,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BV50"/>
+  <dimension ref="A1:CK50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35629,6 +35629,66 @@
           <t>Average</t>
         </is>
       </c>
+      <c r="BX1" s="4" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="BY1" s="4" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="BZ1" s="4" t="inlineStr">
+        <is>
+          <t>Throttle</t>
+        </is>
+      </c>
+      <c r="CA1" s="4" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="CC1" s="4" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="CD1" s="4" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="CE1" s="4" t="inlineStr">
+        <is>
+          <t>Throttle</t>
+        </is>
+      </c>
+      <c r="CF1" s="4" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="CH1" s="4" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="CI1" s="4" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="CJ1" s="4" t="inlineStr">
+        <is>
+          <t>Throttle</t>
+        </is>
+      </c>
+      <c r="CK1" s="4" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -35826,6 +35886,45 @@
         <f>AVERAGE(BT$2:BT$10000)</f>
         <v/>
       </c>
+      <c r="BX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>18.19603</v>
+      </c>
+      <c r="BZ2" t="n">
+        <v>160</v>
+      </c>
+      <c r="CA2">
+        <f>AVERAGE(BY$2:BY$10000)</f>
+        <v/>
+      </c>
+      <c r="CC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>20.52737</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>170</v>
+      </c>
+      <c r="CF2">
+        <f>AVERAGE(CD$2:CD$10000)</f>
+        <v/>
+      </c>
+      <c r="CH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>22.89871</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK2">
+        <f>AVERAGE(CI$2:CI$10000)</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -35963,7 +36062,34 @@
       <c r="BU3" t="n">
         <v>150</v>
       </c>
-      <c r="BV3" t="inlineStr"/>
+      <c r="BX3" t="n">
+        <v>0.1075410842895508</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>18.11602</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC3" t="n">
+        <v>0.1086728572845459</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>20.44008</v>
+      </c>
+      <c r="CE3" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>0.1090800762176514</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>22.86961</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -36101,7 +36227,34 @@
       <c r="BU4" t="n">
         <v>150</v>
       </c>
-      <c r="BV4" t="inlineStr"/>
+      <c r="BX4" t="n">
+        <v>0.2167470455169678</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>18.13784</v>
+      </c>
+      <c r="BZ4" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC4" t="n">
+        <v>0.2231700420379639</v>
+      </c>
+      <c r="CD4" t="n">
+        <v>20.40371</v>
+      </c>
+      <c r="CE4" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH4" t="n">
+        <v>0.2235701084136963</v>
+      </c>
+      <c r="CI4" t="n">
+        <v>22.85143</v>
+      </c>
+      <c r="CJ4" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -36239,7 +36392,34 @@
       <c r="BU5" t="n">
         <v>150</v>
       </c>
-      <c r="BV5" t="inlineStr"/>
+      <c r="BX5" t="n">
+        <v>0.3216550350189209</v>
+      </c>
+      <c r="BY5" t="n">
+        <v>18.12693</v>
+      </c>
+      <c r="BZ5" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC5" t="n">
+        <v>0.3219082355499268</v>
+      </c>
+      <c r="CD5" t="n">
+        <v>20.48372</v>
+      </c>
+      <c r="CE5" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH5" t="n">
+        <v>0.3258321285247803</v>
+      </c>
+      <c r="CI5" t="n">
+        <v>22.68049</v>
+      </c>
+      <c r="CJ5" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -36377,7 +36557,34 @@
       <c r="BU6" t="n">
         <v>150</v>
       </c>
-      <c r="BV6" t="inlineStr"/>
+      <c r="BX6" t="n">
+        <v>0.4226131439208984</v>
+      </c>
+      <c r="BY6" t="n">
+        <v>18.10875</v>
+      </c>
+      <c r="BZ6" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC6" t="n">
+        <v>0.4244990348815918</v>
+      </c>
+      <c r="CD6" t="n">
+        <v>20.60011</v>
+      </c>
+      <c r="CE6" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH6" t="n">
+        <v>0.4244880676269531</v>
+      </c>
+      <c r="CI6" t="n">
+        <v>22.61138</v>
+      </c>
+      <c r="CJ6" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -36515,7 +36722,34 @@
       <c r="BU7" t="n">
         <v>150</v>
       </c>
-      <c r="BV7" t="inlineStr"/>
+      <c r="BX7" t="n">
+        <v>0.5345690250396729</v>
+      </c>
+      <c r="BY7" t="n">
+        <v>17.97418</v>
+      </c>
+      <c r="BZ7" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC7" t="n">
+        <v>0.5393209457397461</v>
+      </c>
+      <c r="CD7" t="n">
+        <v>20.5892</v>
+      </c>
+      <c r="CE7" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH7" t="n">
+        <v>0.5392971038818359</v>
+      </c>
+      <c r="CI7" t="n">
+        <v>22.62229</v>
+      </c>
+      <c r="CJ7" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -36653,7 +36887,34 @@
       <c r="BU8" t="n">
         <v>150</v>
       </c>
-      <c r="BV8" t="inlineStr"/>
+      <c r="BX8" t="n">
+        <v>0.6347250938415527</v>
+      </c>
+      <c r="BY8" t="n">
+        <v>17.90507</v>
+      </c>
+      <c r="BZ8" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC8" t="n">
+        <v>0.6416690349578857</v>
+      </c>
+      <c r="CD8" t="n">
+        <v>20.59647</v>
+      </c>
+      <c r="CE8" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH8" t="n">
+        <v>0.6420822143554688</v>
+      </c>
+      <c r="CI8" t="n">
+        <v>22.65139</v>
+      </c>
+      <c r="CJ8" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -36791,7 +37052,34 @@
       <c r="BU9" t="n">
         <v>150</v>
       </c>
-      <c r="BV9" t="inlineStr"/>
+      <c r="BX9" t="n">
+        <v>0.7363111972808838</v>
+      </c>
+      <c r="BY9" t="n">
+        <v>17.80687</v>
+      </c>
+      <c r="BZ9" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC9" t="n">
+        <v>0.7439918518066406</v>
+      </c>
+      <c r="CD9" t="n">
+        <v>20.66558</v>
+      </c>
+      <c r="CE9" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH9" t="n">
+        <v>0.7424211502075195</v>
+      </c>
+      <c r="CI9" t="n">
+        <v>22.61138</v>
+      </c>
+      <c r="CJ9" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -36929,7 +37217,34 @@
       <c r="BU10" t="n">
         <v>150</v>
       </c>
-      <c r="BV10" t="inlineStr"/>
+      <c r="BX10" t="n">
+        <v>0.8417160511016846</v>
+      </c>
+      <c r="BY10" t="n">
+        <v>17.75596</v>
+      </c>
+      <c r="BZ10" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC10" t="n">
+        <v>0.8428399562835693</v>
+      </c>
+      <c r="CD10" t="n">
+        <v>20.70558</v>
+      </c>
+      <c r="CE10" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH10" t="n">
+        <v>0.8438351154327393</v>
+      </c>
+      <c r="CI10" t="n">
+        <v>22.53864</v>
+      </c>
+      <c r="CJ10" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -37067,7 +37382,34 @@
       <c r="BU11" t="n">
         <v>150</v>
       </c>
-      <c r="BV11" t="inlineStr"/>
+      <c r="BX11" t="n">
+        <v>0.9582200050354004</v>
+      </c>
+      <c r="BY11" t="n">
+        <v>17.78869</v>
+      </c>
+      <c r="BZ11" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC11" t="n">
+        <v>0.957859992980957</v>
+      </c>
+      <c r="CD11" t="n">
+        <v>20.7274</v>
+      </c>
+      <c r="CE11" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH11" t="n">
+        <v>0.9578161239624023</v>
+      </c>
+      <c r="CI11" t="n">
+        <v>22.46954</v>
+      </c>
+      <c r="CJ11" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -37205,7 +37547,34 @@
       <c r="BU12" t="n">
         <v>150</v>
       </c>
-      <c r="BV12" t="inlineStr"/>
+      <c r="BX12" t="n">
+        <v>1.057835102081299</v>
+      </c>
+      <c r="BY12" t="n">
+        <v>17.78505</v>
+      </c>
+      <c r="BZ12" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC12" t="n">
+        <v>1.059904813766479</v>
+      </c>
+      <c r="CD12" t="n">
+        <v>20.64012</v>
+      </c>
+      <c r="CE12" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH12" t="n">
+        <v>1.060455083847046</v>
+      </c>
+      <c r="CI12" t="n">
+        <v>22.44772</v>
+      </c>
+      <c r="CJ12" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -37343,7 +37712,34 @@
       <c r="BU13" t="n">
         <v>150</v>
       </c>
-      <c r="BV13" t="inlineStr"/>
+      <c r="BX13" t="n">
+        <v>1.158406019210815</v>
+      </c>
+      <c r="BY13" t="n">
+        <v>17.74141</v>
+      </c>
+      <c r="BZ13" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC13" t="n">
+        <v>1.162369012832642</v>
+      </c>
+      <c r="CD13" t="n">
+        <v>20.50555</v>
+      </c>
+      <c r="CE13" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH13" t="n">
+        <v>1.162843942642212</v>
+      </c>
+      <c r="CI13" t="n">
+        <v>22.50955</v>
+      </c>
+      <c r="CJ13" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -37481,7 +37877,34 @@
       <c r="BU14" t="n">
         <v>150</v>
       </c>
-      <c r="BV14" t="inlineStr"/>
+      <c r="BX14" t="n">
+        <v>1.273499250411987</v>
+      </c>
+      <c r="BY14" t="n">
+        <v>17.6323</v>
+      </c>
+      <c r="BZ14" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC14" t="n">
+        <v>1.270005941390991</v>
+      </c>
+      <c r="CD14" t="n">
+        <v>20.43644</v>
+      </c>
+      <c r="CE14" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH14" t="n">
+        <v>1.27343225479126</v>
+      </c>
+      <c r="CI14" t="n">
+        <v>22.55683</v>
+      </c>
+      <c r="CJ14" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -37619,7 +38042,34 @@
       <c r="BU15" t="n">
         <v>150</v>
       </c>
-      <c r="BV15" t="inlineStr"/>
+      <c r="BX15" t="n">
+        <v>1.375983238220215</v>
+      </c>
+      <c r="BY15" t="n">
+        <v>17.50136</v>
+      </c>
+      <c r="BZ15" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC15" t="n">
+        <v>1.375956773757935</v>
+      </c>
+      <c r="CD15" t="n">
+        <v>20.45099</v>
+      </c>
+      <c r="CE15" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH15" t="n">
+        <v>1.37645411491394</v>
+      </c>
+      <c r="CI15" t="n">
+        <v>22.60775</v>
+      </c>
+      <c r="CJ15" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -37757,7 +38207,34 @@
       <c r="BU16" t="n">
         <v>150</v>
       </c>
-      <c r="BV16" t="inlineStr"/>
+      <c r="BX16" t="n">
+        <v>1.473496198654175</v>
+      </c>
+      <c r="BY16" t="n">
+        <v>17.37043</v>
+      </c>
+      <c r="BZ16" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC16" t="n">
+        <v>1.47816801071167</v>
+      </c>
+      <c r="CD16" t="n">
+        <v>20.41462</v>
+      </c>
+      <c r="CE16" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH16" t="n">
+        <v>1.478929042816162</v>
+      </c>
+      <c r="CI16" t="n">
+        <v>22.61866</v>
+      </c>
+      <c r="CJ16" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -37895,7 +38372,34 @@
       <c r="BU17" t="n">
         <v>150</v>
       </c>
-      <c r="BV17" t="inlineStr"/>
+      <c r="BX17" t="n">
+        <v>1.578449010848999</v>
+      </c>
+      <c r="BY17" t="n">
+        <v>17.39225</v>
+      </c>
+      <c r="BZ17" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC17" t="n">
+        <v>1.577882051467896</v>
+      </c>
+      <c r="CD17" t="n">
+        <v>20.40007</v>
+      </c>
+      <c r="CE17" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH17" t="n">
+        <v>1.580824136734009</v>
+      </c>
+      <c r="CI17" t="n">
+        <v>22.47318</v>
+      </c>
+      <c r="CJ17" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -38033,7 +38537,34 @@
       <c r="BU18" t="n">
         <v>150</v>
       </c>
-      <c r="BV18" t="inlineStr"/>
+      <c r="BX18" t="n">
+        <v>1.687505006790161</v>
+      </c>
+      <c r="BY18" t="n">
+        <v>17.45772</v>
+      </c>
+      <c r="BZ18" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC18" t="n">
+        <v>1.689548015594482</v>
+      </c>
+      <c r="CD18" t="n">
+        <v>20.35643</v>
+      </c>
+      <c r="CE18" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH18" t="n">
+        <v>1.692317008972168</v>
+      </c>
+      <c r="CI18" t="n">
+        <v>22.38225</v>
+      </c>
+      <c r="CJ18" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -38171,7 +38702,34 @@
       <c r="BU19" t="n">
         <v>150</v>
       </c>
-      <c r="BV19" t="inlineStr"/>
+      <c r="BX19" t="n">
+        <v>1.790419101715088</v>
+      </c>
+      <c r="BY19" t="n">
+        <v>17.41771</v>
+      </c>
+      <c r="BZ19" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC19" t="n">
+        <v>1.794646978378296</v>
+      </c>
+      <c r="CD19" t="n">
+        <v>20.30551</v>
+      </c>
+      <c r="CE19" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH19" t="n">
+        <v>1.795017004013062</v>
+      </c>
+      <c r="CI19" t="n">
+        <v>22.34952</v>
+      </c>
+      <c r="CJ19" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -38309,7 +38867,34 @@
       <c r="BU20" t="n">
         <v>150</v>
       </c>
-      <c r="BV20" t="inlineStr"/>
+      <c r="BX20" t="n">
+        <v>1.8929762840271</v>
+      </c>
+      <c r="BY20" t="n">
+        <v>17.36679</v>
+      </c>
+      <c r="BZ20" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC20" t="n">
+        <v>1.894302129745483</v>
+      </c>
+      <c r="CD20" t="n">
+        <v>20.32369</v>
+      </c>
+      <c r="CE20" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH20" t="n">
+        <v>1.897741079330444</v>
+      </c>
+      <c r="CI20" t="n">
+        <v>22.27314</v>
+      </c>
+      <c r="CJ20" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -38447,7 +39032,34 @@
       <c r="BU21" t="n">
         <v>150</v>
       </c>
-      <c r="BV21" t="inlineStr"/>
+      <c r="BX21" t="n">
+        <v>2.004419088363647</v>
+      </c>
+      <c r="BY21" t="n">
+        <v>17.41044</v>
+      </c>
+      <c r="BZ21" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC21" t="n">
+        <v>2.003628015518188</v>
+      </c>
+      <c r="CD21" t="n">
+        <v>20.33824</v>
+      </c>
+      <c r="CE21" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH21" t="n">
+        <v>2.008318185806274</v>
+      </c>
+      <c r="CI21" t="n">
+        <v>22.33497</v>
+      </c>
+      <c r="CJ21" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -38585,7 +39197,34 @@
       <c r="BU22" t="n">
         <v>150</v>
       </c>
-      <c r="BV22" t="inlineStr"/>
+      <c r="BX22" t="n">
+        <v>2.10674786567688</v>
+      </c>
+      <c r="BY22" t="n">
+        <v>17.43953</v>
+      </c>
+      <c r="BZ22" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC22" t="n">
+        <v>2.110406160354614</v>
+      </c>
+      <c r="CD22" t="n">
+        <v>20.29096</v>
+      </c>
+      <c r="CE22" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH22" t="n">
+        <v>2.110866069793701</v>
+      </c>
+      <c r="CI22" t="n">
+        <v>22.45135</v>
+      </c>
+      <c r="CJ22" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -38723,7 +39362,34 @@
       <c r="BU23" t="n">
         <v>150</v>
       </c>
-      <c r="BV23" t="inlineStr"/>
+      <c r="BX23" t="n">
+        <v>2.212419033050537</v>
+      </c>
+      <c r="BY23" t="n">
+        <v>17.42862</v>
+      </c>
+      <c r="BZ23" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC23" t="n">
+        <v>2.212788820266724</v>
+      </c>
+      <c r="CD23" t="n">
+        <v>20.18185</v>
+      </c>
+      <c r="CE23" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH23" t="n">
+        <v>2.213197231292725</v>
+      </c>
+      <c r="CI23" t="n">
+        <v>22.55319</v>
+      </c>
+      <c r="CJ23" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -38861,7 +39527,34 @@
       <c r="BU24" t="n">
         <v>150</v>
       </c>
-      <c r="BV24" t="inlineStr"/>
+      <c r="BX24" t="n">
+        <v>2.315145015716553</v>
+      </c>
+      <c r="BY24" t="n">
+        <v>17.42862</v>
+      </c>
+      <c r="BZ24" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC24" t="n">
+        <v>2.316333055496216</v>
+      </c>
+      <c r="CD24" t="n">
+        <v>20.04364</v>
+      </c>
+      <c r="CE24" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH24" t="n">
+        <v>2.315363883972168</v>
+      </c>
+      <c r="CI24" t="n">
+        <v>22.52409</v>
+      </c>
+      <c r="CJ24" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -38999,7 +39692,34 @@
       <c r="BU25" t="n">
         <v>150</v>
       </c>
-      <c r="BV25" t="inlineStr"/>
+      <c r="BX25" t="n">
+        <v>2.42632007598877</v>
+      </c>
+      <c r="BY25" t="n">
+        <v>17.53046</v>
+      </c>
+      <c r="BZ25" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC25" t="n">
+        <v>2.426781177520752</v>
+      </c>
+      <c r="CD25" t="n">
+        <v>20.01091</v>
+      </c>
+      <c r="CE25" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH25" t="n">
+        <v>2.427615165710449</v>
+      </c>
+      <c r="CI25" t="n">
+        <v>22.38589</v>
+      </c>
+      <c r="CJ25" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -39137,7 +39857,34 @@
       <c r="BU26" t="n">
         <v>150</v>
       </c>
-      <c r="BV26" t="inlineStr"/>
+      <c r="BX26" t="n">
+        <v>2.526144027709961</v>
+      </c>
+      <c r="BY26" t="n">
+        <v>17.52319</v>
+      </c>
+      <c r="BZ26" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC26" t="n">
+        <v>2.529526948928833</v>
+      </c>
+      <c r="CD26" t="n">
+        <v>20.02182</v>
+      </c>
+      <c r="CE26" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH26" t="n">
+        <v>2.530019998550415</v>
+      </c>
+      <c r="CI26" t="n">
+        <v>22.31315</v>
+      </c>
+      <c r="CJ26" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -39275,7 +40022,34 @@
       <c r="BU27" t="n">
         <v>150</v>
       </c>
-      <c r="BV27" t="inlineStr"/>
+      <c r="BX27" t="n">
+        <v>2.627568244934082</v>
+      </c>
+      <c r="BY27" t="n">
+        <v>17.57047</v>
+      </c>
+      <c r="BZ27" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC27" t="n">
+        <v>2.632133960723877</v>
+      </c>
+      <c r="CD27" t="n">
+        <v>19.97454</v>
+      </c>
+      <c r="CE27" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH27" t="n">
+        <v>2.631734132766724</v>
+      </c>
+      <c r="CI27" t="n">
+        <v>22.23313</v>
+      </c>
+      <c r="CJ27" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -39413,7 +40187,34 @@
       <c r="BU28" t="n">
         <v>150</v>
       </c>
-      <c r="BV28" t="inlineStr"/>
+      <c r="BX28" t="n">
+        <v>2.736038208007812</v>
+      </c>
+      <c r="BY28" t="n">
+        <v>17.7014</v>
+      </c>
+      <c r="BZ28" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC28" t="n">
+        <v>2.741067886352539</v>
+      </c>
+      <c r="CD28" t="n">
+        <v>19.90544</v>
+      </c>
+      <c r="CE28" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH28" t="n">
+        <v>2.745681047439575</v>
+      </c>
+      <c r="CI28" t="n">
+        <v>22.18949</v>
+      </c>
+      <c r="CJ28" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -39551,7 +40352,34 @@
       <c r="BU29" t="n">
         <v>150</v>
       </c>
-      <c r="BV29" t="inlineStr"/>
+      <c r="BX29" t="n">
+        <v>2.84304404258728</v>
+      </c>
+      <c r="BY29" t="n">
+        <v>17.78141</v>
+      </c>
+      <c r="BZ29" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC29" t="n">
+        <v>2.845823049545288</v>
+      </c>
+      <c r="CD29" t="n">
+        <v>19.82906</v>
+      </c>
+      <c r="CE29" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH29" t="n">
+        <v>2.847625017166138</v>
+      </c>
+      <c r="CI29" t="n">
+        <v>22.10947</v>
+      </c>
+      <c r="CJ29" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -39689,7 +40517,34 @@
       <c r="BU30" t="n">
         <v>150</v>
       </c>
-      <c r="BV30" t="inlineStr"/>
+      <c r="BX30" t="n">
+        <v>2.94780707359314</v>
+      </c>
+      <c r="BY30" t="n">
+        <v>17.83233</v>
+      </c>
+      <c r="BZ30" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC30" t="n">
+        <v>2.947897911071777</v>
+      </c>
+      <c r="CD30" t="n">
+        <v>19.86543</v>
+      </c>
+      <c r="CE30" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH30" t="n">
+        <v>2.94667911529541</v>
+      </c>
+      <c r="CI30" t="n">
+        <v>21.99309</v>
+      </c>
+      <c r="CJ30" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -39827,7 +40682,34 @@
       <c r="BU31" t="n">
         <v>150</v>
       </c>
-      <c r="BV31" t="inlineStr"/>
+      <c r="BX31" t="n">
+        <v>3.044317960739136</v>
+      </c>
+      <c r="BY31" t="n">
+        <v>17.80687</v>
+      </c>
+      <c r="BZ31" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC31" t="n">
+        <v>3.047083854675293</v>
+      </c>
+      <c r="CD31" t="n">
+        <v>19.94544</v>
+      </c>
+      <c r="CE31" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH31" t="n">
+        <v>3.049187898635864</v>
+      </c>
+      <c r="CI31" t="n">
+        <v>21.9058</v>
+      </c>
+      <c r="CJ31" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -39965,7 +40847,34 @@
       <c r="BU32" t="n">
         <v>150</v>
       </c>
-      <c r="BV32" t="inlineStr"/>
+      <c r="BX32" t="n">
+        <v>3.158737897872925</v>
+      </c>
+      <c r="BY32" t="n">
+        <v>17.83961</v>
+      </c>
+      <c r="BZ32" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC32" t="n">
+        <v>3.162883996963501</v>
+      </c>
+      <c r="CD32" t="n">
+        <v>19.9709</v>
+      </c>
+      <c r="CE32" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH32" t="n">
+        <v>3.162238121032715</v>
+      </c>
+      <c r="CI32" t="n">
+        <v>21.86579</v>
+      </c>
+      <c r="CJ32" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -40103,7 +41012,34 @@
       <c r="BU33" t="n">
         <v>150</v>
       </c>
-      <c r="BV33" t="inlineStr"/>
+      <c r="BX33" t="n">
+        <v>3.2621910572052</v>
+      </c>
+      <c r="BY33" t="n">
+        <v>17.93781</v>
+      </c>
+      <c r="BZ33" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC33" t="n">
+        <v>3.263036966323853</v>
+      </c>
+      <c r="CD33" t="n">
+        <v>19.91271</v>
+      </c>
+      <c r="CE33" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH33" t="n">
+        <v>3.267028093338013</v>
+      </c>
+      <c r="CI33" t="n">
+        <v>21.86579</v>
+      </c>
+      <c r="CJ33" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -40241,7 +41177,34 @@
       <c r="BU34" t="n">
         <v>150</v>
       </c>
-      <c r="BV34" t="inlineStr"/>
+      <c r="BX34" t="n">
+        <v>3.364587068557739</v>
+      </c>
+      <c r="BY34" t="n">
+        <v>18.04692</v>
+      </c>
+      <c r="BZ34" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC34" t="n">
+        <v>3.364655017852783</v>
+      </c>
+      <c r="CD34" t="n">
+        <v>19.8727</v>
+      </c>
+      <c r="CE34" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH34" t="n">
+        <v>3.370543956756592</v>
+      </c>
+      <c r="CI34" t="n">
+        <v>21.9349</v>
+      </c>
+      <c r="CJ34" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -40379,7 +41342,34 @@
       <c r="BU35" t="n">
         <v>150</v>
       </c>
-      <c r="BV35" t="inlineStr"/>
+      <c r="BX35" t="n">
+        <v>3.480756998062134</v>
+      </c>
+      <c r="BY35" t="n">
+        <v>18.0251</v>
+      </c>
+      <c r="BZ35" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC35" t="n">
+        <v>3.47959303855896</v>
+      </c>
+      <c r="CD35" t="n">
+        <v>19.87634</v>
+      </c>
+      <c r="CE35" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH35" t="n">
+        <v>3.480432987213135</v>
+      </c>
+      <c r="CI35" t="n">
+        <v>22.05492</v>
+      </c>
+      <c r="CJ35" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -40517,7 +41507,34 @@
       <c r="BU36" t="n">
         <v>150</v>
       </c>
-      <c r="BV36" t="inlineStr"/>
+      <c r="BX36" t="n">
+        <v>3.579766035079956</v>
+      </c>
+      <c r="BY36" t="n">
+        <v>17.93417</v>
+      </c>
+      <c r="BZ36" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC36" t="n">
+        <v>3.583679914474487</v>
+      </c>
+      <c r="CD36" t="n">
+        <v>19.9309</v>
+      </c>
+      <c r="CE36" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH36" t="n">
+        <v>3.583847045898438</v>
+      </c>
+      <c r="CI36" t="n">
+        <v>22.11675</v>
+      </c>
+      <c r="CJ36" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -40655,7 +41672,34 @@
       <c r="BU37" t="n">
         <v>150</v>
       </c>
-      <c r="BV37" t="inlineStr"/>
+      <c r="BX37" t="n">
+        <v>3.680719137191772</v>
+      </c>
+      <c r="BY37" t="n">
+        <v>17.93781</v>
+      </c>
+      <c r="BZ37" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC37" t="n">
+        <v>3.686292886734009</v>
+      </c>
+      <c r="CD37" t="n">
+        <v>20.01091</v>
+      </c>
+      <c r="CE37" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH37" t="n">
+        <v>3.685561895370483</v>
+      </c>
+      <c r="CI37" t="n">
+        <v>22.17494</v>
+      </c>
+      <c r="CJ37" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -40793,7 +41837,34 @@
       <c r="BU38" t="n">
         <v>150</v>
       </c>
-      <c r="BV38" t="inlineStr"/>
+      <c r="BX38" t="n">
+        <v>3.78402304649353</v>
+      </c>
+      <c r="BY38" t="n">
+        <v>18.04328</v>
+      </c>
+      <c r="BZ38" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC38" t="n">
+        <v>3.786252975463867</v>
+      </c>
+      <c r="CD38" t="n">
+        <v>20.06183</v>
+      </c>
+      <c r="CE38" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH38" t="n">
+        <v>3.788429260253906</v>
+      </c>
+      <c r="CI38" t="n">
+        <v>22.20767</v>
+      </c>
+      <c r="CJ38" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -40931,7 +42002,34 @@
       <c r="BU39" t="n">
         <v>150</v>
       </c>
-      <c r="BV39" t="inlineStr"/>
+      <c r="BX39" t="n">
+        <v>3.899835109710693</v>
+      </c>
+      <c r="BY39" t="n">
+        <v>18.1233</v>
+      </c>
+      <c r="BZ39" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC39" t="n">
+        <v>3.899373054504395</v>
+      </c>
+      <c r="CD39" t="n">
+        <v>20.05455</v>
+      </c>
+      <c r="CE39" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH39" t="n">
+        <v>3.895135164260864</v>
+      </c>
+      <c r="CI39" t="n">
+        <v>22.17858</v>
+      </c>
+      <c r="CJ39" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -41069,7 +42167,34 @@
       <c r="BU40" t="n">
         <v>150</v>
       </c>
-      <c r="BV40" t="inlineStr"/>
+      <c r="BX40" t="n">
+        <v>3.996761083602905</v>
+      </c>
+      <c r="BY40" t="n">
+        <v>18.11602</v>
+      </c>
+      <c r="BZ40" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC40" t="n">
+        <v>4.001857995986938</v>
+      </c>
+      <c r="CD40" t="n">
+        <v>20.08729</v>
+      </c>
+      <c r="CE40" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH40" t="n">
+        <v>4.002155065536499</v>
+      </c>
+      <c r="CI40" t="n">
+        <v>22.2004</v>
+      </c>
+      <c r="CJ40" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -41207,7 +42332,34 @@
       <c r="BU41" t="n">
         <v>150</v>
       </c>
-      <c r="BV41" t="inlineStr"/>
+      <c r="BX41" t="n">
+        <v>4.097466230392456</v>
+      </c>
+      <c r="BY41" t="n">
+        <v>18.17058</v>
+      </c>
+      <c r="BZ41" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC41" t="n">
+        <v>4.10199499130249</v>
+      </c>
+      <c r="CD41" t="n">
+        <v>20.17821</v>
+      </c>
+      <c r="CE41" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH41" t="n">
+        <v>4.098201274871826</v>
+      </c>
+      <c r="CI41" t="n">
+        <v>22.17858</v>
+      </c>
+      <c r="CJ41" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -41345,7 +42497,34 @@
       <c r="BU42" t="n">
         <v>150</v>
       </c>
-      <c r="BV42" t="inlineStr"/>
+      <c r="BX42" t="n">
+        <v>4.217478036880493</v>
+      </c>
+      <c r="BY42" t="n">
+        <v>18.21786</v>
+      </c>
+      <c r="BZ42" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC42" t="n">
+        <v>4.213370084762573</v>
+      </c>
+      <c r="CD42" t="n">
+        <v>20.30551</v>
+      </c>
+      <c r="CE42" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH42" t="n">
+        <v>4.214606285095215</v>
+      </c>
+      <c r="CI42" t="n">
+        <v>22.20767</v>
+      </c>
+      <c r="CJ42" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -41483,7 +42662,34 @@
       <c r="BU43" t="n">
         <v>150</v>
       </c>
-      <c r="BV43" t="inlineStr"/>
+      <c r="BX43" t="n">
+        <v>4.309432029724121</v>
+      </c>
+      <c r="BY43" t="n">
+        <v>18.23968</v>
+      </c>
+      <c r="BZ43" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC43" t="n">
+        <v>4.318670034408569</v>
+      </c>
+      <c r="CD43" t="n">
+        <v>20.35279</v>
+      </c>
+      <c r="CE43" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH43" t="n">
+        <v>4.316421985626221</v>
+      </c>
+      <c r="CI43" t="n">
+        <v>22.25859</v>
+      </c>
+      <c r="CJ43" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -41621,7 +42827,34 @@
       <c r="BU44" t="n">
         <v>150</v>
       </c>
-      <c r="BV44" t="inlineStr"/>
+      <c r="BX44" t="n">
+        <v>4.416725158691406</v>
+      </c>
+      <c r="BY44" t="n">
+        <v>18.34515</v>
+      </c>
+      <c r="BZ44" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC44" t="n">
+        <v>4.420450925827026</v>
+      </c>
+      <c r="CD44" t="n">
+        <v>20.3346</v>
+      </c>
+      <c r="CE44" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH44" t="n">
+        <v>4.420114040374756</v>
+      </c>
+      <c r="CI44" t="n">
+        <v>22.28041</v>
+      </c>
+      <c r="CJ44" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -41759,7 +42992,34 @@
       <c r="BU45" t="n">
         <v>150</v>
       </c>
-      <c r="BV45" t="inlineStr"/>
+      <c r="BX45" t="n">
+        <v>4.527283906936646</v>
+      </c>
+      <c r="BY45" t="n">
+        <v>18.46154</v>
+      </c>
+      <c r="BZ45" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC45" t="n">
+        <v>4.525115966796875</v>
+      </c>
+      <c r="CD45" t="n">
+        <v>20.34915</v>
+      </c>
+      <c r="CE45" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH45" t="n">
+        <v>4.523087978363037</v>
+      </c>
+      <c r="CI45" t="n">
+        <v>22.2695</v>
+      </c>
+      <c r="CJ45" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -41897,7 +43157,34 @@
       <c r="BU46" t="n">
         <v>150</v>
       </c>
-      <c r="BV46" t="inlineStr"/>
+      <c r="BX46" t="n">
+        <v>4.627026081085205</v>
+      </c>
+      <c r="BY46" t="n">
+        <v>18.48336</v>
+      </c>
+      <c r="BZ46" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC46" t="n">
+        <v>4.635289907455444</v>
+      </c>
+      <c r="CD46" t="n">
+        <v>20.45099</v>
+      </c>
+      <c r="CE46" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH46" t="n">
+        <v>4.633004188537598</v>
+      </c>
+      <c r="CI46" t="n">
+        <v>22.31315</v>
+      </c>
+      <c r="CJ46" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -42035,7 +43322,34 @@
       <c r="BU47" t="n">
         <v>150</v>
       </c>
-      <c r="BV47" t="inlineStr"/>
+      <c r="BX47" t="n">
+        <v>4.728835105895996</v>
+      </c>
+      <c r="BY47" t="n">
+        <v>18.46881</v>
+      </c>
+      <c r="BZ47" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC47" t="n">
+        <v>4.731697082519531</v>
+      </c>
+      <c r="CD47" t="n">
+        <v>20.50191</v>
+      </c>
+      <c r="CE47" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH47" t="n">
+        <v>4.737190961837769</v>
+      </c>
+      <c r="CI47" t="n">
+        <v>22.30224</v>
+      </c>
+      <c r="CJ47" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -42173,7 +43487,34 @@
       <c r="BU48" t="n">
         <v>150</v>
       </c>
-      <c r="BV48" t="inlineStr"/>
+      <c r="BX48" t="n">
+        <v>4.837996006011963</v>
+      </c>
+      <c r="BY48" t="n">
+        <v>18.47245</v>
+      </c>
+      <c r="BZ48" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC48" t="n">
+        <v>4.836639165878296</v>
+      </c>
+      <c r="CD48" t="n">
+        <v>20.47645</v>
+      </c>
+      <c r="CE48" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH48" t="n">
+        <v>4.838066101074219</v>
+      </c>
+      <c r="CI48" t="n">
+        <v>22.30224</v>
+      </c>
+      <c r="CJ48" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -42311,7 +43652,34 @@
       <c r="BU49" t="n">
         <v>150</v>
       </c>
-      <c r="BV49" t="inlineStr"/>
+      <c r="BX49" t="n">
+        <v>4.949648857116699</v>
+      </c>
+      <c r="BY49" t="n">
+        <v>18.49063</v>
+      </c>
+      <c r="BZ49" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC49" t="n">
+        <v>4.946612119674683</v>
+      </c>
+      <c r="CD49" t="n">
+        <v>20.36734</v>
+      </c>
+      <c r="CE49" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH49" t="n">
+        <v>4.949712038040161</v>
+      </c>
+      <c r="CI49" t="n">
+        <v>22.33133</v>
+      </c>
+      <c r="CJ49" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -42449,7 +43817,34 @@
       <c r="BU50" t="n">
         <v>150</v>
       </c>
-      <c r="BV50" t="inlineStr"/>
+      <c r="BX50" t="n">
+        <v>5.044745922088623</v>
+      </c>
+      <c r="BY50" t="n">
+        <v>18.55974</v>
+      </c>
+      <c r="BZ50" t="n">
+        <v>160</v>
+      </c>
+      <c r="CC50" t="n">
+        <v>5.052932977676392</v>
+      </c>
+      <c r="CD50" t="n">
+        <v>20.25823</v>
+      </c>
+      <c r="CE50" t="n">
+        <v>170</v>
+      </c>
+      <c r="CH50" t="n">
+        <v>5.052811145782471</v>
+      </c>
+      <c r="CI50" t="n">
+        <v>22.27314</v>
+      </c>
+      <c r="CJ50" t="n">
+        <v>180</v>
+      </c>
+      <c r="CK50" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>